<commit_message>
fix: update flash map
</commit_message>
<xml_diff>
--- a/doc/tl_ble_mesh_flash_map.xlsx
+++ b/doc/tl_ble_mesh_flash_map.xlsx
@@ -1,16 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="637"/>
+    <workbookView windowWidth="22188" windowHeight="10500" tabRatio="637"/>
   </bookViews>
   <sheets>
     <sheet name="SIGMeshB91m1M" sheetId="15" r:id="rId1"/>
     <sheet name="tl321xRAM_map" sheetId="16" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,49 +116,49 @@
     <t>FLASH_ADR_MD_LIGHT_LC</t>
   </si>
   <si>
+    <t>FLASH_ADR_MD_DF_SBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Parameters </t>
+  </si>
+  <si>
+    <t>For User define</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MD_LIGHTNESS</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MISC</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MD_SENSOR</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_RESET_CNT</t>
+  </si>
+  <si>
+    <t>Hardware Secure BootDecriptor(16K)</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MD_LIGHT_HSL</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_SW_LEVEL</t>
+  </si>
+  <si>
+    <t>reserved for telink</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MD_G_POWER_ONOFF</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MD_MISC_PAR</t>
+  </si>
+  <si>
+    <t>FLASH_ADR_MD_PROPERTY</t>
+  </si>
+  <si>
     <t>FLASH_ADR_VC_NODE_INFO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Parameters </t>
-  </si>
-  <si>
-    <t>For User define</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_LIGHTNESS</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_DF_SBR</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_SENSOR</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MISC</t>
-  </si>
-  <si>
-    <t>Hardware Secure BootDecriptor(16K)</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_LIGHT_HSL</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_RESET_CNT</t>
-  </si>
-  <si>
-    <t>reserved for telink</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_G_POWER_ONOFF</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_SW_LEVEL</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_MISC_PAR</t>
-  </si>
-  <si>
-    <t>FLASH_ADR_MD_PROPERTY</t>
   </si>
   <si>
     <t>FLASH_ADR_MESH_TYPE_FLAG</t>
@@ -227,7 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -291,34 +304,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -332,14 +317,6 @@
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -379,6 +356,21 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -429,7 +421,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,91 +565,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,21 +790,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -820,6 +818,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,153 +891,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1046,9 +1059,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1106,19 +1116,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1268,52 +1269,52 @@
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
     <cellStyle name="常规 2" xfId="49"/>
@@ -1330,6 +1331,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1593,860 +1601,860 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="9.25" style="11" customWidth="1"/>
-    <col min="3" max="3" width="30.6333333333333" customWidth="1"/>
+    <col min="2" max="2" width="9.25" style="10" customWidth="1"/>
+    <col min="3" max="3" width="30.6296296296296" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="32.425" customWidth="1"/>
-    <col min="6" max="6" width="5.63333333333333" customWidth="1"/>
+    <col min="5" max="5" width="32.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="5.62962962962963" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="9.88333333333333" style="11" customWidth="1"/>
-    <col min="9" max="9" width="35.1333333333333" customWidth="1"/>
-    <col min="10" max="10" width="10.3833333333333" customWidth="1"/>
-    <col min="12" max="12" width="9.11666666666667" customWidth="1"/>
-    <col min="13" max="13" width="31.1333333333333" customWidth="1"/>
+    <col min="8" max="8" width="9.87962962962963" style="10" customWidth="1"/>
+    <col min="9" max="9" width="35.1296296296296" customWidth="1"/>
+    <col min="10" max="10" width="10.3796296296296" customWidth="1"/>
+    <col min="12" max="12" width="9.12037037037037" customWidth="1"/>
+    <col min="13" max="13" width="31.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="39" customHeight="1" spans="2:14">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="H1" s="11" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" ht="23.25" customHeight="1" spans="1:14">
       <c r="A2" s="5"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="I2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="12" t="s">
+      <c r="M2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:14">
-      <c r="A3" s="14" t="s">
+    <row r="3" ht="15.6" spans="1:14">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>384</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="H3" s="15">
+      <c r="E3" s="17"/>
+      <c r="H3" s="14">
         <v>60000</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="45">
-        <v>4</v>
-      </c>
-      <c r="L3" s="15" t="s">
+      <c r="J3" s="41">
+        <v>4</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="M3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:14">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20" t="s">
+      <c r="N3" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" ht="15.6" spans="1:14">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="14"/>
-      <c r="H4" s="21" t="str">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="13"/>
+      <c r="H4" s="20" t="str">
         <f t="shared" ref="H4:H8" si="0">DEC2HEX(HEX2DEC(H3)+J3*1024-1)</f>
         <v>60FFF</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
-      <c r="L4" s="21" t="str">
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
+      <c r="L4" s="20" t="str">
         <f t="shared" ref="L4:L8" si="1">DEC2HEX(HEX2DEC(L3)+N3*1024-1)</f>
         <v>E0FFF</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="48"/>
-    </row>
-    <row r="5" ht="15.75" spans="1:14">
-      <c r="A5" s="19"/>
-      <c r="B5" s="21" t="str">
+      <c r="M4" s="45"/>
+      <c r="N4" s="44"/>
+    </row>
+    <row r="5" ht="15.6" spans="1:14">
+      <c r="A5" s="18"/>
+      <c r="B5" s="20" t="str">
         <f>DEC2HEX(HEX2DEC(B3)+D3*1024-1)</f>
         <v>5FFFF</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="14"/>
-      <c r="H5" s="15" t="str">
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="13"/>
+      <c r="H5" s="14" t="str">
         <f t="shared" ref="H5:H9" si="2">DEC2HEX(HEX2DEC(H4)+1)</f>
         <v>61000</v>
       </c>
-      <c r="I5" s="50" t="s">
+      <c r="I5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="45">
-        <v>4</v>
-      </c>
-      <c r="L5" s="15" t="str">
+      <c r="J5" s="41">
+        <v>4</v>
+      </c>
+      <c r="L5" s="14" t="str">
         <f t="shared" ref="L5:L9" si="3">DEC2HEX(HEX2DEC(L4)+1)</f>
         <v>E1000</v>
       </c>
-      <c r="M5" s="51" t="s">
+      <c r="M5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:14">
-      <c r="A6" s="19"/>
-      <c r="B6" s="15" t="str">
+      <c r="N5" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" ht="15.6" spans="1:14">
+      <c r="A6" s="18"/>
+      <c r="B6" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B5)+1)</f>
         <v>60000</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>128</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="21" t="str">
+      <c r="H6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>61FFF</v>
       </c>
-      <c r="I6" s="52"/>
-      <c r="J6" s="48"/>
-      <c r="L6" s="21" t="str">
+      <c r="I6" s="48"/>
+      <c r="J6" s="44"/>
+      <c r="L6" s="20" t="str">
         <f t="shared" si="1"/>
         <v>E1FFF</v>
       </c>
-      <c r="M6" s="53"/>
-      <c r="N6" s="48"/>
-    </row>
-    <row r="7" ht="15.75" spans="1:14">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20" t="s">
+      <c r="M6" s="49"/>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" ht="15.6" spans="1:14">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="H7" s="15" t="str">
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="8"/>
+      <c r="H7" s="14" t="str">
         <f t="shared" si="2"/>
         <v>62000</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="45">
-        <v>4</v>
-      </c>
-      <c r="L7" s="15" t="str">
+      <c r="J7" s="41">
+        <v>4</v>
+      </c>
+      <c r="L7" s="14" t="str">
         <f t="shared" si="3"/>
         <v>E2000</v>
       </c>
-      <c r="M7" s="55" t="s">
+      <c r="M7" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:14">
-      <c r="A8" s="19"/>
-      <c r="B8" s="21" t="str">
+      <c r="N7" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" ht="15.6" spans="1:14">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20" t="str">
         <f>DEC2HEX(HEX2DEC(B6)+D6*1024-1)</f>
         <v>7FFFF</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="H8" s="21" t="str">
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="9"/>
+      <c r="H8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>62FFF</v>
       </c>
-      <c r="I8" s="56"/>
-      <c r="J8" s="48"/>
-      <c r="L8" s="21" t="str">
+      <c r="I8" s="52"/>
+      <c r="J8" s="44"/>
+      <c r="L8" s="20" t="str">
         <f t="shared" si="1"/>
         <v>E2FFF</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="48"/>
-    </row>
-    <row r="9" ht="15.75" spans="1:14">
-      <c r="A9" s="19"/>
-      <c r="B9" s="15" t="str">
+      <c r="M8" s="53"/>
+      <c r="N8" s="44"/>
+    </row>
+    <row r="9" ht="15.6" spans="1:14">
+      <c r="A9" s="18"/>
+      <c r="B9" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B8)+1)</f>
         <v>80000</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>384</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="H9" s="15" t="str">
+      <c r="E9" s="7"/>
+      <c r="H9" s="14" t="str">
         <f t="shared" si="2"/>
         <v>63000</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="45">
-        <v>4</v>
-      </c>
-      <c r="L9" s="15" t="str">
+      <c r="J9" s="41">
+        <v>4</v>
+      </c>
+      <c r="L9" s="14" t="str">
         <f t="shared" si="3"/>
         <v>E3000</v>
       </c>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" spans="1:14">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20" t="s">
+      <c r="N9" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" ht="15.6" spans="1:14">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="H10" s="21" t="str">
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="8"/>
+      <c r="H10" s="20" t="str">
         <f t="shared" ref="H10:H14" si="4">DEC2HEX(HEX2DEC(H9)+J9*1024-1)</f>
         <v>63FFF</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="48"/>
-      <c r="L10" s="21" t="str">
+      <c r="I10" s="56"/>
+      <c r="J10" s="44"/>
+      <c r="L10" s="20" t="str">
         <f t="shared" ref="L10:L14" si="5">DEC2HEX(HEX2DEC(L9)+N9*1024-1)</f>
         <v>E3FFF</v>
       </c>
-      <c r="M10" s="61"/>
-      <c r="N10" s="48"/>
-    </row>
-    <row r="11" ht="15.75" spans="1:14">
-      <c r="A11" s="19"/>
-      <c r="B11" s="21" t="str">
+      <c r="M10" s="57"/>
+      <c r="N10" s="44"/>
+    </row>
+    <row r="11" ht="15.6" spans="1:14">
+      <c r="A11" s="18"/>
+      <c r="B11" s="20" t="str">
         <f>DEC2HEX(HEX2DEC(B9)+D9*1024-1)</f>
         <v>DFFFF</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="30"/>
-      <c r="H11" s="15" t="str">
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="9"/>
+      <c r="H11" s="14" t="str">
         <f t="shared" ref="H11:H15" si="6">DEC2HEX(HEX2DEC(H10)+1)</f>
         <v>64000</v>
       </c>
-      <c r="I11" s="62" t="s">
+      <c r="I11" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="45">
-        <v>4</v>
-      </c>
-      <c r="L11" s="15" t="str">
+      <c r="J11" s="41">
+        <v>4</v>
+      </c>
+      <c r="L11" s="14" t="str">
         <f t="shared" ref="L11:L15" si="7">DEC2HEX(HEX2DEC(L10)+1)</f>
         <v>E4000</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" spans="1:14">
+      <c r="N11" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" ht="15.6" spans="1:14">
       <c r="A12" s="3"/>
-      <c r="B12" s="32" t="str">
+      <c r="B12" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B11)+1)</f>
         <v>E0000</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>64</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="21" t="str">
+      <c r="H12" s="20" t="str">
         <f t="shared" si="4"/>
         <v>64FFF</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="48"/>
-      <c r="L12" s="21" t="str">
+      <c r="I12" s="59"/>
+      <c r="J12" s="44"/>
+      <c r="L12" s="20" t="str">
         <f t="shared" si="5"/>
         <v>E4FFF</v>
       </c>
-      <c r="M12" s="61"/>
-      <c r="N12" s="48"/>
-    </row>
-    <row r="13" ht="15.75" spans="1:14">
+      <c r="M12" s="57"/>
+      <c r="N12" s="44"/>
+    </row>
+    <row r="13" ht="15.6" spans="1:14">
       <c r="A13" s="3"/>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="H13" s="15" t="str">
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="8"/>
+      <c r="H13" s="14" t="str">
         <f t="shared" si="6"/>
         <v>65000</v>
       </c>
-      <c r="I13" s="64" t="s">
+      <c r="I13" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="45">
-        <v>4</v>
-      </c>
-      <c r="L13" s="15" t="str">
+      <c r="J13" s="41">
+        <v>4</v>
+      </c>
+      <c r="L13" s="14" t="str">
         <f t="shared" si="7"/>
         <v>E5000</v>
       </c>
-      <c r="M13" s="65" t="s">
+      <c r="M13" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="N13" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" spans="1:14">
+      <c r="N13" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" ht="15.6" spans="1:14">
       <c r="A14" s="3"/>
-      <c r="B14" s="34" t="str">
+      <c r="B14" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B12)+D12*1024-1)</f>
         <v>EFFFF</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="H14" s="21" t="str">
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="9"/>
+      <c r="H14" s="20" t="str">
         <f t="shared" si="4"/>
         <v>65FFF</v>
       </c>
-      <c r="I14" s="66"/>
-      <c r="J14" s="48"/>
-      <c r="L14" s="21" t="str">
+      <c r="I14" s="62"/>
+      <c r="J14" s="44"/>
+      <c r="L14" s="20" t="str">
         <f t="shared" si="5"/>
         <v>E5FFF</v>
       </c>
-      <c r="M14" s="67"/>
-      <c r="N14" s="48"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="44"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:14">
       <c r="A15" s="3"/>
-      <c r="B15" s="32" t="str">
+      <c r="B15" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B14)+1)</f>
         <v>F0000</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="22">
         <v>32</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="15" t="str">
+      <c r="H15" s="14" t="str">
         <f t="shared" si="6"/>
         <v>66000</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="45">
-        <v>4</v>
-      </c>
-      <c r="L15" s="15" t="str">
+      <c r="J15" s="41">
+        <v>4</v>
+      </c>
+      <c r="L15" s="14" t="str">
         <f t="shared" si="7"/>
         <v>E6000</v>
       </c>
-      <c r="M15" s="68" t="s">
+      <c r="M15" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="N15" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" spans="1:14">
+      <c r="N15" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" ht="15.6" spans="1:14">
       <c r="A16" s="3"/>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="H16" s="21" t="str">
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="8"/>
+      <c r="H16" s="20" t="str">
         <f t="shared" ref="H16:H20" si="8">DEC2HEX(HEX2DEC(H15)+J15*1024-1)</f>
         <v>66FFF</v>
       </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="48"/>
-      <c r="L16" s="21" t="str">
+      <c r="I16" s="53"/>
+      <c r="J16" s="44"/>
+      <c r="L16" s="20" t="str">
         <f t="shared" ref="L16:L20" si="9">DEC2HEX(HEX2DEC(L15)+N15*1024-1)</f>
         <v>E6FFF</v>
       </c>
-      <c r="M16" s="69"/>
-      <c r="N16" s="48"/>
-    </row>
-    <row r="17" ht="15.75" spans="1:14">
+      <c r="M16" s="65"/>
+      <c r="N16" s="44"/>
+    </row>
+    <row r="17" ht="15.6" spans="1:14">
       <c r="A17" s="3"/>
-      <c r="B17" s="34" t="str">
+      <c r="B17" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B15)+D15*1024-1)</f>
         <v>F7FFF</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-      <c r="H17" s="15" t="str">
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="9"/>
+      <c r="H17" s="14" t="str">
         <f t="shared" ref="H17:H21" si="10">DEC2HEX(HEX2DEC(H16)+1)</f>
         <v>67000</v>
       </c>
-      <c r="I17" s="70" t="s">
+      <c r="I17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="45">
-        <v>4</v>
-      </c>
-      <c r="L17" s="15" t="str">
+      <c r="J17" s="41">
+        <v>4</v>
+      </c>
+      <c r="L17" s="14" t="str">
         <f t="shared" ref="L17:L21" si="11">DEC2HEX(HEX2DEC(L16)+1)</f>
         <v>E7000</v>
       </c>
-      <c r="M17" s="71" t="s">
+      <c r="M17" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="N17" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" spans="1:14">
+      <c r="N17" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" ht="15.6" spans="1:14">
       <c r="A18" s="3"/>
-      <c r="B18" s="32" t="str">
+      <c r="B18" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B17)+1)</f>
         <v>F8000</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>16</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="H18" s="21" t="str">
+      <c r="E18" s="7"/>
+      <c r="H18" s="20" t="str">
         <f t="shared" si="8"/>
         <v>67FFF</v>
       </c>
-      <c r="I18" s="72"/>
-      <c r="J18" s="48"/>
-      <c r="L18" s="21" t="str">
+      <c r="I18" s="68"/>
+      <c r="J18" s="44"/>
+      <c r="L18" s="20" t="str">
         <f t="shared" si="9"/>
         <v>E7FFF</v>
       </c>
-      <c r="M18" s="28"/>
-      <c r="N18" s="48"/>
-    </row>
-    <row r="19" ht="15.75" spans="1:14">
+      <c r="M18" s="26"/>
+      <c r="N18" s="44"/>
+    </row>
+    <row r="19" ht="15.6" spans="1:14">
       <c r="A19" s="3"/>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="H19" s="15" t="str">
+      <c r="C19" s="32"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="8"/>
+      <c r="H19" s="14" t="str">
         <f t="shared" si="10"/>
         <v>68000</v>
       </c>
-      <c r="I19" s="73" t="s">
+      <c r="I19" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="J19" s="45">
-        <v>4</v>
-      </c>
-      <c r="L19" s="15" t="str">
+      <c r="J19" s="41">
+        <v>4</v>
+      </c>
+      <c r="L19" s="14" t="str">
         <f t="shared" si="11"/>
         <v>E8000</v>
       </c>
-      <c r="M19" s="55" t="s">
+      <c r="M19" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" spans="1:14">
+      <c r="N19" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" ht="15.6" spans="1:14">
       <c r="A20" s="3"/>
-      <c r="B20" s="34" t="str">
+      <c r="B20" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B18)+D18*1024-1)</f>
         <v>FBFFF</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="H20" s="21" t="str">
+      <c r="C20" s="33"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="9"/>
+      <c r="H20" s="20" t="str">
         <f t="shared" si="8"/>
         <v>68FFF</v>
       </c>
-      <c r="I20" s="74"/>
-      <c r="J20" s="48"/>
-      <c r="L20" s="21" t="str">
+      <c r="I20" s="70"/>
+      <c r="J20" s="44"/>
+      <c r="L20" s="20" t="str">
         <f t="shared" si="9"/>
         <v>E8FFF</v>
       </c>
-      <c r="M20" s="57"/>
-      <c r="N20" s="48"/>
-    </row>
-    <row r="21" ht="15.75" spans="1:14">
+      <c r="M20" s="53"/>
+      <c r="N20" s="44"/>
+    </row>
+    <row r="21" ht="15.6" spans="1:14">
       <c r="A21" s="3"/>
-      <c r="B21" s="32" t="str">
+      <c r="B21" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B20)+1)</f>
         <v>FC000</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="23">
-        <v>4</v>
-      </c>
-      <c r="E21" s="31"/>
-      <c r="H21" s="15" t="str">
+      <c r="D21" s="22">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="H21" s="14" t="str">
         <f t="shared" si="10"/>
         <v>69000</v>
       </c>
-      <c r="I21" s="75" t="s">
+      <c r="I21" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="J21" s="45">
-        <v>4</v>
-      </c>
-      <c r="L21" s="15" t="str">
+      <c r="J21" s="41">
+        <v>4</v>
+      </c>
+      <c r="L21" s="14" t="str">
         <f t="shared" si="11"/>
         <v>E9000</v>
       </c>
-      <c r="M21" s="71" t="s">
+      <c r="M21" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="N21" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" spans="1:14">
+      <c r="N21" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" ht="15.6" spans="1:14">
       <c r="A22" s="3"/>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="H22" s="21" t="str">
+      <c r="C22" s="35"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="8"/>
+      <c r="H22" s="20" t="str">
         <f t="shared" ref="H22:H26" si="12">DEC2HEX(HEX2DEC(H21)+J21*1024-1)</f>
         <v>69FFF</v>
       </c>
-      <c r="I22" s="76"/>
-      <c r="J22" s="48"/>
-      <c r="L22" s="21" t="str">
+      <c r="I22" s="72"/>
+      <c r="J22" s="44"/>
+      <c r="L22" s="20" t="str">
         <f t="shared" ref="L22:L26" si="13">DEC2HEX(HEX2DEC(L21)+N21*1024-1)</f>
         <v>E9FFF</v>
       </c>
-      <c r="M22" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="N22" s="48"/>
-    </row>
-    <row r="23" ht="15.75" spans="1:14">
+      <c r="M22" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" s="44"/>
+    </row>
+    <row r="23" ht="15.6" spans="1:14">
       <c r="A23" s="3"/>
-      <c r="B23" s="34" t="str">
+      <c r="B23" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B21)+D21*1024-1)</f>
         <v>FCFFF</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="H23" s="15" t="str">
+      <c r="C23" s="36"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="9"/>
+      <c r="H23" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(H22)+1)</f>
         <v>6A000</v>
       </c>
-      <c r="I23" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="45">
-        <v>4</v>
-      </c>
-      <c r="L23" s="15" t="str">
+      <c r="I23" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="41">
+        <v>4</v>
+      </c>
+      <c r="L23" s="14" t="str">
         <f t="shared" ref="L23:L27" si="14">DEC2HEX(HEX2DEC(L22)+1)</f>
         <v>EA000</v>
       </c>
-      <c r="M23" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="N23" s="45">
+      <c r="M23" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="41">
         <v>8</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="1:14">
+    <row r="24" ht="15.6" spans="1:14">
       <c r="A24" s="3"/>
-      <c r="B24" s="32" t="str">
+      <c r="B24" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B23)+1)</f>
         <v>FD000</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="23">
-        <v>4</v>
-      </c>
-      <c r="E24" s="31" t="s">
+      <c r="D24" s="22">
+        <v>4</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="21" t="str">
+      <c r="H24" s="20" t="str">
         <f t="shared" si="12"/>
         <v>6AFFF</v>
       </c>
-      <c r="I24" s="76"/>
-      <c r="J24" s="48"/>
-      <c r="L24" s="21" t="str">
+      <c r="I24" s="72"/>
+      <c r="J24" s="44"/>
+      <c r="L24" s="20" t="str">
         <f t="shared" si="13"/>
         <v>EBFFF</v>
       </c>
-      <c r="M24" s="57"/>
-      <c r="N24" s="48"/>
-    </row>
-    <row r="25" ht="15.75" spans="1:14">
+      <c r="M24" s="53"/>
+      <c r="N24" s="44"/>
+    </row>
+    <row r="25" ht="15.6" spans="1:14">
       <c r="A25" s="3"/>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="H25" s="15" t="str">
+      <c r="C25" s="35"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="8"/>
+      <c r="H25" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(H24)+1)</f>
         <v>6B000</v>
       </c>
-      <c r="I25" s="77" t="s">
+      <c r="I25" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="J25" s="45">
-        <v>4</v>
-      </c>
-      <c r="L25" s="15" t="str">
+      <c r="J25" s="41">
+        <v>4</v>
+      </c>
+      <c r="L25" s="14" t="str">
         <f t="shared" si="14"/>
         <v>EC000</v>
       </c>
-      <c r="M25" s="55" t="s">
+      <c r="M25" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="N25" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" spans="1:14">
+      <c r="N25" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" ht="15.6" spans="1:14">
       <c r="A26" s="3"/>
-      <c r="B26" s="34" t="str">
+      <c r="B26" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B24)+D24*1024-1)</f>
         <v>FDFFF</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="H26" s="21" t="str">
+      <c r="C26" s="36"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="9"/>
+      <c r="H26" s="20" t="str">
         <f t="shared" si="12"/>
         <v>6BFFF</v>
       </c>
-      <c r="I26" s="78"/>
-      <c r="J26" s="48"/>
-      <c r="L26" s="21" t="str">
+      <c r="I26" s="74"/>
+      <c r="J26" s="44"/>
+      <c r="L26" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>ECFFF</v>
-      </c>
-      <c r="M26" s="57"/>
-      <c r="N26" s="48"/>
+        <v>EDFFF</v>
+      </c>
+      <c r="M26" s="53"/>
+      <c r="N26" s="44"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="1:14">
       <c r="A27" s="3"/>
-      <c r="B27" s="32" t="str">
+      <c r="B27" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B26)+1)</f>
         <v>FE000</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="23">
-        <v>4</v>
-      </c>
-      <c r="E27" s="31" t="s">
+      <c r="D27" s="22">
+        <v>4</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>48</v>
       </c>
       <c r="H27"/>
-      <c r="L27" s="15" t="str">
-        <f t="shared" si="14"/>
-        <v>ED000</v>
-      </c>
-      <c r="M27" s="55" t="s">
+      <c r="L27" s="14" t="str">
+        <f>DEC2HEX(HEX2DEC(L26)+1)</f>
+        <v>EE000</v>
+      </c>
+      <c r="M27" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="N27" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" spans="1:14">
+      <c r="N27" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" ht="15.6" spans="1:14">
       <c r="A28" s="3"/>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="8"/>
       <c r="H28"/>
-      <c r="L28" s="21" t="str">
+      <c r="L28" s="20" t="str">
         <f>DEC2HEX(HEX2DEC(L27)+N27*1024-1)</f>
-        <v>EDFFF</v>
-      </c>
-      <c r="M28" s="57"/>
-      <c r="N28" s="48"/>
-    </row>
-    <row r="29" ht="15.75" spans="1:14">
+        <v>EEFFF</v>
+      </c>
+      <c r="M28" s="53"/>
+      <c r="N28" s="44"/>
+    </row>
+    <row r="29" ht="15.6" spans="1:14">
       <c r="A29" s="3"/>
-      <c r="B29" s="34" t="str">
+      <c r="B29" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B27)+D27*1024-1)</f>
         <v>FEFFF</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="9"/>
       <c r="H29"/>
-      <c r="L29" s="15" t="str">
+      <c r="L29" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(L28)+1)</f>
-        <v>EE000</v>
-      </c>
-      <c r="M29" s="55" t="s">
+        <v>EF000</v>
+      </c>
+      <c r="M29" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="45">
+      <c r="N29" s="41">
         <v>4</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:14">
       <c r="A30" s="3"/>
-      <c r="B30" s="32" t="str">
+      <c r="B30" s="28" t="str">
         <f>DEC2HEX(HEX2DEC(B29)+1)</f>
         <v>FF000</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="23">
-        <v>4</v>
-      </c>
-      <c r="E30" s="31"/>
+      <c r="D30" s="22">
+        <v>4</v>
+      </c>
+      <c r="E30" s="7"/>
       <c r="H30"/>
-      <c r="L30" s="21" t="str">
+      <c r="L30" s="20" t="str">
         <f>DEC2HEX(HEX2DEC(L29)+N29*1024-1)</f>
-        <v>EEFFF</v>
-      </c>
-      <c r="M30" s="57"/>
-      <c r="N30" s="48"/>
+        <v>EFFFF</v>
+      </c>
+      <c r="M30" s="53"/>
+      <c r="N30" s="44"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:8">
       <c r="A31" s="3"/>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="8"/>
       <c r="H31"/>
     </row>
     <row r="32" ht="14.25" customHeight="1" spans="1:8">
       <c r="A32" s="3"/>
-      <c r="B32" s="34" t="str">
+      <c r="B32" s="30" t="str">
         <f>DEC2HEX(HEX2DEC(B30)+D30*1024-1)</f>
         <v>FFFFF</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="9"/>
       <c r="H32"/>
     </row>
     <row r="33" spans="5:8">
-      <c r="E33" s="42"/>
+      <c r="E33" s="38"/>
       <c r="H33"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="43"/>
-      <c r="E34" s="42"/>
+      <c r="B34" s="39"/>
+      <c r="E34" s="38"/>
       <c r="H34"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" spans="5:8">
-      <c r="E35" s="42"/>
+      <c r="E35" s="38"/>
       <c r="H35"/>
     </row>
     <row r="36" spans="5:5">
-      <c r="E36" s="42"/>
+      <c r="E36" s="38"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="42"/>
+      <c r="E37" s="38"/>
     </row>
     <row r="38" spans="5:5">
-      <c r="E38" s="42"/>
+      <c r="E38" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="87">
@@ -2553,10 +2561,10 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="19.1333333333333" customWidth="1"/>
+    <col min="2" max="2" width="19.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2730,7 +2738,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2739,7 +2747,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1"/>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="1"/>
@@ -2752,7 +2760,7 @@
       <c r="A20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C20" s="1"/>
@@ -2763,7 +2771,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="4"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="1"/>
@@ -2774,7 +2782,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1"/>
-      <c r="B22" s="9"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2783,7 +2791,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1"/>
-      <c r="B23" s="10"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2792,7 +2800,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1"/>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="1"/>
@@ -2803,7 +2811,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1"/>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="1"/>

</xml_diff>